<commit_message>
v0.15 Bolletjes 5 punten
</commit_message>
<xml_diff>
--- a/tdf-2024.xlsx
+++ b/tdf-2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\CODE\Tourploeg\Claude\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E532D3CA-59D2-4547-927B-1EE0C7C4E165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0759A901-37D5-477A-870E-CA37E70AFF93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="1" xr2:uid="{C407EA6E-0DA1-4649-9E9C-17974BBC531D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" activeTab="4" xr2:uid="{C407EA6E-0DA1-4649-9E9C-17974BBC531D}"/>
   </bookViews>
   <sheets>
     <sheet name="Renners" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1216" uniqueCount="351">
   <si>
     <t>Renner</t>
   </si>
@@ -442,43 +442,10 @@
     <t>Markus Hoelgaard</t>
   </si>
   <si>
-    <t>Categorie</t>
-  </si>
-  <si>
     <t>Positie</t>
   </si>
   <si>
     <t>Punten</t>
-  </si>
-  <si>
-    <t>Eindklassement</t>
-  </si>
-  <si>
-    <t>Trui Groen</t>
-  </si>
-  <si>
-    <t>Trui Bolletjes</t>
-  </si>
-  <si>
-    <t>Trui Wit</t>
-  </si>
-  <si>
-    <t>Etappe</t>
-  </si>
-  <si>
-    <t>Trui</t>
-  </si>
-  <si>
-    <t>Geel</t>
-  </si>
-  <si>
-    <t>Groen</t>
-  </si>
-  <si>
-    <t>Bolletjes</t>
-  </si>
-  <si>
-    <t>Wit</t>
   </si>
   <si>
     <t>Adriaan Mutter</t>
@@ -1692,7 +1659,7 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -1702,17 +1669,17 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -1722,22 +1689,22 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -1747,7 +1714,7 @@
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
@@ -1757,12 +1724,12 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
@@ -1772,12 +1739,12 @@
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
@@ -1787,7 +1754,7 @@
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
@@ -1797,7 +1764,7 @@
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
@@ -1807,12 +1774,12 @@
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
@@ -1822,22 +1789,22 @@
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
@@ -1852,22 +1819,22 @@
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
@@ -1877,7 +1844,7 @@
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
@@ -1892,12 +1859,12 @@
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
@@ -1917,7 +1884,7 @@
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
@@ -1932,7 +1899,7 @@
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
@@ -1942,17 +1909,17 @@
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -1967,7 +1934,7 @@
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
@@ -1977,7 +1944,7 @@
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
@@ -1987,7 +1954,7 @@
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
@@ -1997,12 +1964,12 @@
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
@@ -2012,17 +1979,17 @@
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
@@ -2047,7 +2014,7 @@
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
@@ -2057,12 +2024,12 @@
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
@@ -2072,7 +2039,7 @@
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
@@ -2082,17 +2049,17 @@
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
@@ -2102,7 +2069,7 @@
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
@@ -2112,7 +2079,7 @@
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
@@ -2137,17 +2104,17 @@
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
@@ -2157,12 +2124,12 @@
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
@@ -2177,17 +2144,17 @@
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
@@ -2212,27 +2179,27 @@
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
@@ -2242,7 +2209,7 @@
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
@@ -2252,17 +2219,17 @@
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
@@ -2272,22 +2239,22 @@
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>356</v>
+        <v>345</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
@@ -2297,17 +2264,17 @@
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
@@ -2322,7 +2289,7 @@
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
@@ -2332,7 +2299,7 @@
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
@@ -2342,7 +2309,7 @@
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
@@ -2352,17 +2319,17 @@
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
@@ -2377,12 +2344,12 @@
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
@@ -2392,22 +2359,22 @@
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
@@ -2417,22 +2384,22 @@
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>302</v>
+        <v>291</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
@@ -2442,7 +2409,7 @@
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
@@ -2452,22 +2419,22 @@
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
@@ -2477,7 +2444,7 @@
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
@@ -2487,7 +2454,7 @@
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
@@ -2502,12 +2469,12 @@
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
@@ -2522,17 +2489,17 @@
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
@@ -2542,12 +2509,12 @@
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
     </row>
   </sheetData>
@@ -2562,7 +2529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{612D4934-4074-44C7-907B-E3C3A3F4753F}">
   <dimension ref="A1:A36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -2573,7 +2540,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -2593,22 +2560,22 @@
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -2618,7 +2585,7 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
@@ -2628,7 +2595,7 @@
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
@@ -2638,12 +2605,12 @@
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
@@ -2663,52 +2630,52 @@
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
@@ -2723,32 +2690,32 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -2818,139 +2785,139 @@
   <sheetData>
     <row r="1" spans="1:45" s="5" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="O1" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="R1" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="U1" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="H1" s="6" t="s">
+      <c r="V1" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="W1" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="X1" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>242</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="Y1" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="Z1" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="AA1" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="AB1" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="Q1" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="R1" s="6" t="s">
+      <c r="AC1" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="AD1" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="T1" s="6" t="s">
+      <c r="AE1" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="U1" s="6" t="s">
+      <c r="AF1" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="AG1" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="AH1" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="V1" s="6" t="s">
+      <c r="AI1" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="W1" s="6" t="s">
+      <c r="AJ1" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="AK1" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="X1" s="6" t="s">
+      <c r="AL1" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="AM1" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="Y1" s="6" t="s">
+      <c r="AN1" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="Z1" s="6" t="s">
+      <c r="AO1" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="AA1" s="6" t="s">
+      <c r="AP1" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="AB1" s="6" t="s">
+      <c r="AQ1" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="AC1" s="6" t="s">
+      <c r="AR1" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="AD1" s="6" t="s">
+      <c r="AS1" s="6" t="s">
         <v>165</v>
-      </c>
-      <c r="AE1" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="AF1" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="AG1" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="AH1" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="AI1" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="AJ1" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="AK1" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="AL1" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="AM1" s="6" t="s">
-        <v>170</v>
-      </c>
-      <c r="AN1" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="AO1" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="AP1" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="AQ1" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="AR1" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="AS1" s="6" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.25">
@@ -4605,181 +4572,135 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136BDC3E-BED0-409D-967D-A99BB8EAFC9D}">
   <sheetPr codeName="Blad3"/>
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12:C15"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>134</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>134</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
       </c>
       <c r="B3" s="2">
-        <v>2</v>
-      </c>
-      <c r="C3" s="2">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>134</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
       </c>
       <c r="B4" s="2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
         <v>3</v>
       </c>
-      <c r="C4" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B5" s="2">
-        <v>4</v>
-      </c>
-      <c r="C5" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="2">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="B12" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="B13" s="2">
         <v>5</v>
       </c>
-      <c r="C6" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B7" s="2">
-        <v>6</v>
-      </c>
-      <c r="C7" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B8" s="2">
-        <v>7</v>
-      </c>
-      <c r="C8" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B9" s="2">
-        <v>8</v>
-      </c>
-      <c r="C9" s="2">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B14" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B10" s="2">
-        <v>9</v>
-      </c>
-      <c r="C10" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11" s="2">
-        <v>10</v>
-      </c>
-      <c r="C11" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="C12" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="C14" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="C15" s="2">
+        <v>189</v>
+      </c>
+      <c r="B15" s="2">
         <v>3</v>
       </c>
     </row>
@@ -4791,346 +4712,255 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0135B218-F896-485E-9C84-4836B4354BB2}">
   <sheetPr codeName="Blad4"/>
-  <dimension ref="A1:C30"/>
+  <dimension ref="A1:B30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>127</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
-        <v>130</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
-      </c>
-      <c r="C2" s="4">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>130</v>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4">
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>130</v>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>130</v>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>4</v>
-      </c>
-      <c r="C5" s="4">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>130</v>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>5</v>
-      </c>
-      <c r="C6" s="4">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>130</v>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>6</v>
-      </c>
-      <c r="C7" s="4">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>130</v>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>7</v>
-      </c>
-      <c r="C8" s="4">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>130</v>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>8</v>
-      </c>
-      <c r="C9" s="4">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>130</v>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>9</v>
-      </c>
-      <c r="C10" s="4">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>130</v>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>130</v>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="4">
+        <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>11</v>
-      </c>
-      <c r="C12" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>130</v>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="4">
+        <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>130</v>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="4">
+        <v>13</v>
       </c>
       <c r="B14" s="4">
-        <v>13</v>
-      </c>
-      <c r="C14" s="4">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>130</v>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="4">
+        <v>14</v>
       </c>
       <c r="B15" s="4">
-        <v>14</v>
-      </c>
-      <c r="C15" s="4">
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>130</v>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="4">
+        <v>15</v>
       </c>
       <c r="B16" s="4">
         <v>15</v>
       </c>
-      <c r="C16" s="4">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>130</v>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="4">
+        <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>16</v>
-      </c>
-      <c r="C17" s="4">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>130</v>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>17</v>
-      </c>
-      <c r="C18" s="4">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>130</v>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="4">
+        <v>18</v>
       </c>
       <c r="B19" s="4">
-        <v>18</v>
-      </c>
-      <c r="C19" s="4">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>130</v>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4">
+        <v>19</v>
       </c>
       <c r="B20" s="4">
-        <v>19</v>
-      </c>
-      <c r="C20" s="4">
         <v>11</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>130</v>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="4">
+        <v>20</v>
       </c>
       <c r="B21" s="4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B22" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B23" s="4">
         <v>20</v>
       </c>
-      <c r="C21" s="4">
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="B24" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" s="4">
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B23" s="4">
-        <v>2</v>
-      </c>
-      <c r="C23" s="4">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="B26" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B24" s="4">
-        <v>3</v>
-      </c>
-      <c r="C24" s="4">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B27" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B26" s="4">
-        <v>2</v>
-      </c>
-      <c r="C26" s="4">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="B28" s="4">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B27" s="4">
-        <v>3</v>
-      </c>
-      <c r="C27" s="4">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="B29" s="4">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B28" s="4">
-        <v>1</v>
-      </c>
-      <c r="C28" s="4">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B29" s="4">
-        <v>2</v>
-      </c>
-      <c r="C29" s="4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>133</v>
+        <v>194</v>
       </c>
       <c r="B30" s="4">
-        <v>3</v>
-      </c>
-      <c r="C30" s="4">
         <v>5</v>
       </c>
     </row>
@@ -5144,7 +4974,7 @@
   <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5181,78 +5011,78 @@
         <v>2024</v>
       </c>
       <c r="B1" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="M1" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="N1" s="13" t="s">
         <v>178</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="O1" s="13" t="s">
         <v>179</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="P1" s="13" t="s">
         <v>180</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="Q1" s="13" t="s">
         <v>181</v>
       </c>
-      <c r="G1" s="13" t="s">
+      <c r="R1" s="13" t="s">
         <v>182</v>
       </c>
-      <c r="H1" s="13" t="s">
+      <c r="S1" s="13" t="s">
         <v>183</v>
       </c>
-      <c r="I1" s="13" t="s">
+      <c r="T1" s="13" t="s">
         <v>184</v>
       </c>
-      <c r="J1" s="13" t="s">
+      <c r="U1" s="13" t="s">
         <v>185</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="V1" s="13" t="s">
         <v>186</v>
       </c>
-      <c r="L1" s="13" t="s">
-        <v>187</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>189</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>190</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>195</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>197</v>
-      </c>
       <c r="W1" s="24" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="X1" s="24" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" spans="1:24" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="23" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="B2" s="22">
         <v>45472</v>
@@ -5326,70 +5156,70 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="B3" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="I3" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>210</v>
-      </c>
-      <c r="D3" s="12" t="s">
+      <c r="J3" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="K3" s="12" t="s">
         <v>211</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="L3" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="M3" s="12" t="s">
         <v>213</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="N3" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="O3" s="12" t="s">
         <v>215</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="P3" s="12" t="s">
         <v>216</v>
       </c>
-      <c r="H3" s="12" t="s">
+      <c r="Q3" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="R3" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="S3" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="T3" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="K3" s="12" t="s">
+      <c r="U3" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="V3" s="12" t="s">
         <v>222</v>
-      </c>
-      <c r="L3" s="12" t="s">
-        <v>223</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>224</v>
-      </c>
-      <c r="N3" s="12" t="s">
-        <v>225</v>
-      </c>
-      <c r="O3" s="12" t="s">
-        <v>226</v>
-      </c>
-      <c r="P3" s="12" t="s">
-        <v>227</v>
-      </c>
-      <c r="Q3" s="12" t="s">
-        <v>228</v>
-      </c>
-      <c r="R3" s="12" t="s">
-        <v>229</v>
-      </c>
-      <c r="S3" s="12" t="s">
-        <v>230</v>
-      </c>
-      <c r="T3" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="U3" s="12" t="s">
-        <v>232</v>
-      </c>
-      <c r="V3" s="12" t="s">
-        <v>233</v>
       </c>
       <c r="W3" s="13">
         <v>2</v>
@@ -5400,7 +5230,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="B4" s="18">
         <v>206</v>
@@ -5474,76 +5304,76 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="G5" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="I5" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="J5" s="12" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="K5" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="L5" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="M5" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="N5" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="O5" s="12" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="P5" s="12" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="Q5" s="12" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="R5" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="T5" s="12" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="V5" s="12" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="W5" s="13">
         <v>4</v>
       </c>
       <c r="X5" s="10" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -5551,7 +5381,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>33</v>
@@ -5563,7 +5393,7 @@
         <v>88</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>83</v>
@@ -5575,7 +5405,7 @@
         <v>13</v>
       </c>
       <c r="J6" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>10</v>
@@ -5617,7 +5447,7 @@
         <v>5</v>
       </c>
       <c r="X6" s="10" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -5649,7 +5479,7 @@
         <v>10</v>
       </c>
       <c r="J7" s="12" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="K7" s="12" t="s">
         <v>13</v>
@@ -5658,10 +5488,10 @@
         <v>88</v>
       </c>
       <c r="M7" s="12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="N7" s="12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="O7" s="12" t="s">
         <v>1</v>
@@ -5676,7 +5506,7 @@
         <v>3</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="T7" s="12" t="s">
         <v>5</v>
@@ -5699,19 +5529,19 @@
         <v>3</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>109</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="G8" s="12" t="s">
         <v>68</v>
@@ -5723,7 +5553,7 @@
         <v>109</v>
       </c>
       <c r="J8" s="12" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="K8" s="12" t="s">
         <v>103</v>
@@ -5744,7 +5574,7 @@
         <v>21</v>
       </c>
       <c r="Q8" s="12" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="R8" s="12" t="s">
         <v>67</v>
@@ -5776,10 +5606,10 @@
         <v>88</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>74</v>
@@ -5800,7 +5630,7 @@
         <v>41</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="L9" s="12" t="s">
         <v>74</v>
@@ -5815,16 +5645,16 @@
         <v>53</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="Q9" s="12" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="R9" s="12" t="s">
         <v>58</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="T9" s="12" t="s">
         <v>44</v>
@@ -5847,7 +5677,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>99</v>
@@ -5859,7 +5689,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="G10" s="12" t="s">
         <v>109</v>
@@ -5868,7 +5698,7 @@
         <v>7</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>45</v>
@@ -5877,28 +5707,28 @@
         <v>68</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="M10" s="12" t="s">
         <v>109</v>
       </c>
       <c r="N10" s="12" t="s">
-        <v>286</v>
+        <v>275</v>
       </c>
       <c r="O10" s="12" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="R10" s="12" t="s">
         <v>31</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>285</v>
+        <v>274</v>
       </c>
       <c r="T10" s="12" t="s">
         <v>21</v>
@@ -5907,13 +5737,13 @@
         <v>67</v>
       </c>
       <c r="V10" s="12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="W10" s="13">
         <v>9</v>
       </c>
       <c r="X10" s="10" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -5936,25 +5766,25 @@
         <v>103</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="H11" s="12" t="s">
         <v>33</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="L11" s="12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="M11" s="12" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="N11" s="12" t="s">
         <v>62</v>
@@ -5972,16 +5802,16 @@
         <v>49</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
       <c r="T11" s="12" t="s">
         <v>1</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="V11" s="12" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="W11" s="13">
         <v>10</v>
@@ -5995,34 +5825,34 @@
         <v>7</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="H12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="J12" s="12" t="s">
         <v>72</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="L12" s="12" t="s">
         <v>90</v>
@@ -6031,7 +5861,7 @@
         <v>37</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="O12" s="12" t="s">
         <v>90</v>
@@ -6040,7 +5870,7 @@
         <v>35</v>
       </c>
       <c r="Q12" s="12" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="R12" s="12" t="s">
         <v>119</v>
@@ -6049,19 +5879,19 @@
         <v>107</v>
       </c>
       <c r="T12" s="12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="U12" s="12" t="s">
         <v>5</v>
       </c>
       <c r="V12" s="12" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="W12" s="11">
         <v>11</v>
       </c>
       <c r="X12" s="10" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -6075,22 +5905,22 @@
         <v>96</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>275</v>
+        <v>264</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="J13" s="12" t="s">
         <v>62</v>
@@ -6099,13 +5929,13 @@
         <v>37</v>
       </c>
       <c r="L13" s="12" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="N13" s="12" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="O13" s="12" t="s">
         <v>43</v>
@@ -6114,19 +5944,19 @@
         <v>53</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="R13" s="12" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="V13" s="12" t="s">
         <v>99</v>
@@ -6143,16 +5973,16 @@
         <v>9</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="F14" s="12" t="s">
         <v>13</v>
@@ -6188,16 +6018,16 @@
         <v>44</v>
       </c>
       <c r="Q14" s="12" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="R14" s="12" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="S14" s="12" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="T14" s="12" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="U14" s="12" t="s">
         <v>90</v>
@@ -6223,40 +6053,40 @@
         <v>44</v>
       </c>
       <c r="D15" s="16" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
       <c r="E15" s="16" t="s">
         <v>35</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="G15" s="16" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="H15" s="16" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="I15" s="16" t="s">
         <v>21</v>
       </c>
       <c r="J15" s="16" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="K15" s="16" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="L15" s="16" t="s">
         <v>43</v>
       </c>
       <c r="M15" s="16" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="N15" s="16" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="O15" s="16" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="P15" s="16" t="s">
         <v>43</v>
@@ -6268,13 +6098,13 @@
         <v>41</v>
       </c>
       <c r="S15" s="16" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="T15" s="16" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="U15" s="16" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="V15" s="16" t="s">
         <v>90</v>
@@ -6288,10 +6118,10 @@
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>88</v>
@@ -6360,7 +6190,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>30</v>
@@ -6427,12 +6257,12 @@
         <v>16</v>
       </c>
       <c r="X17" s="10" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
       <c r="B18" s="12" t="s">
         <v>125</v>
@@ -6504,7 +6334,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="B19" s="12" t="s">
         <v>30</v>
@@ -6571,7 +6401,7 @@
         <v>18</v>
       </c>
       <c r="X19" s="10" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
@@ -6631,7 +6461,7 @@
         <v>20</v>
       </c>
       <c r="X21" s="10" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
@@ -6658,7 +6488,7 @@
       <c r="U22" s="12"/>
       <c r="V22" s="11"/>
       <c r="W22" s="11" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="X22" s="10" t="s">
         <v>13</v>
@@ -6688,7 +6518,7 @@
       <c r="U23" s="12"/>
       <c r="V23" s="11"/>
       <c r="W23" s="11" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="X23" s="10" t="s">
         <v>10</v>
@@ -6718,10 +6548,10 @@
       <c r="U24" s="12"/>
       <c r="V24" s="11"/>
       <c r="W24" s="11" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="X24" s="10" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
@@ -6748,7 +6578,7 @@
       <c r="U25" s="12"/>
       <c r="V25" s="11"/>
       <c r="W25" s="11" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="X25" s="10" t="s">
         <v>44</v>
@@ -6778,7 +6608,7 @@
       <c r="U26" s="12"/>
       <c r="V26" s="11"/>
       <c r="W26" s="11" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="X26" s="10" t="s">
         <v>88</v>
@@ -6808,7 +6638,7 @@
       <c r="U27" s="12"/>
       <c r="V27" s="11"/>
       <c r="W27" s="11" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="X27" s="10" t="s">
         <v>1</v>
@@ -6838,7 +6668,7 @@
       <c r="U28" s="12"/>
       <c r="V28" s="11"/>
       <c r="W28" s="11" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="X28" s="10" t="s">
         <v>21</v>
@@ -6868,7 +6698,7 @@
       <c r="U29" s="12"/>
       <c r="V29" s="11"/>
       <c r="W29" s="11" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="X29" s="10" t="s">
         <v>53</v>
@@ -6898,7 +6728,7 @@
       <c r="U30" s="12"/>
       <c r="V30" s="11"/>
       <c r="W30" s="11" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="X30" s="10" t="s">
         <v>5</v>

</xml_diff>